<commit_message>
added rules metadata for #1 and #2
</commit_message>
<xml_diff>
--- a/rules/CAA_RULES_COMBO.xlsx
+++ b/rules/CAA_RULES_COMBO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="310" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="310" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Rules1" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="129">
   <si>
     <t>Rule #</t>
   </si>
@@ -356,6 +356,33 @@
   </si>
   <si>
     <t>DS-QMW-TN-0010 Page 4 (2.2)</t>
+  </si>
+  <si>
+    <t>Rule-Number</t>
+  </si>
+  <si>
+    <t>Scope</t>
+  </si>
+  <si>
+    <t>Keyword</t>
+  </si>
+  <si>
+    <t>Data-type</t>
+  </si>
+  <si>
+    <t>Cardinality</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Error-Type</t>
+  </si>
+  <si>
+    <t>Error-Message</t>
+  </si>
+  <si>
+    <t>Caveats</t>
   </si>
   <si>
     <t>GLOBAL</t>
@@ -584,7 +611,7 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -617,16 +644,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A16" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A:A"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E64" activeCellId="0" pane="topLeft" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.9540816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.9540816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="16.9540816326531"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.0969387755102"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.94897959183674"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.0510204081633"/>
@@ -636,99 +662,85 @@
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.35" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="2">
+      <c r="E1" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.35" outlineLevel="0" r="2">
       <c r="A2" s="1" t="n">
-        <v>1.01</v>
+        <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="3">
       <c r="A3" s="1" t="n">
-        <v>1.02</v>
+        <v>1.01</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="4">
+      <c r="A4" s="1" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="37.3" outlineLevel="0" r="4">
-      <c r="A4" s="1" t="n">
-        <v>1.03</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="37.3" outlineLevel="0" r="5">
       <c r="A5" s="1" t="n">
-        <v>1.04</v>
+        <v>1.03</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="37.3" outlineLevel="0" r="6">
+      <c r="A6" s="1" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="49.25" outlineLevel="0" r="6">
-      <c r="A6" s="1" t="n">
-        <v>1.05</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="49.25" outlineLevel="0" r="7">
       <c r="A7" s="1" t="n">
-        <v>1.06</v>
+        <v>1.05</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>1</v>
@@ -737,21 +749,18 @@
         <v>11</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="108.95" outlineLevel="0" r="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="49.25" outlineLevel="0" r="8">
       <c r="A8" s="1" t="n">
-        <v>1.07</v>
+        <v>1.06</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>1</v>
@@ -760,43 +769,49 @@
         <v>11</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="108.95" outlineLevel="0" r="9">
+      <c r="A9" s="1" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="9">
-      <c r="A9" s="1" t="n">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="10">
+      <c r="A10" s="1" t="n">
         <v>1.08</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="49.25" outlineLevel="0" r="10">
-      <c r="A10" s="1" t="n">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="49.25" outlineLevel="0" r="11">
+      <c r="A11" s="1" t="n">
         <v>1.09</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="85.05" outlineLevel="0" r="11">
-      <c r="A11" s="1" t="n">
-        <v>1.1</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>22</v>
@@ -805,12 +820,15 @@
         <v>11</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="61.15" outlineLevel="0" r="12">
+        <v>23</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="85.05" outlineLevel="0" r="12">
       <c r="A12" s="1" t="n">
-        <v>1.11</v>
+        <v>1.1</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>22</v>
@@ -818,13 +836,13 @@
       <c r="C12" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="37.3" outlineLevel="0" r="13">
+      <c r="E12" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="61.15" outlineLevel="0" r="13">
       <c r="A13" s="1" t="n">
-        <v>1.12</v>
+        <v>1.11</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>22</v>
@@ -833,12 +851,12 @@
         <v>11</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="49.25" outlineLevel="0" r="14">
+        <v>26</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="37.3" outlineLevel="0" r="14">
       <c r="A14" s="1" t="n">
-        <v>1.13</v>
+        <v>1.12</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>22</v>
@@ -847,14 +865,12 @@
         <v>11</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.35" outlineLevel="0" r="15">
+        <v>27</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="49.25" outlineLevel="0" r="15">
       <c r="A15" s="1" t="n">
-        <v>1.14</v>
+        <v>1.13</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>22</v>
@@ -863,12 +879,14 @@
         <v>11</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="49.25" outlineLevel="0" r="16">
+        <v>28</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.35" outlineLevel="0" r="16">
       <c r="A16" s="1" t="n">
-        <v>1.15</v>
+        <v>1.14</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>22</v>
@@ -877,12 +895,12 @@
         <v>11</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="108.95" outlineLevel="0" r="17">
+        <v>29</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="49.25" outlineLevel="0" r="17">
       <c r="A17" s="1" t="n">
-        <v>1.16</v>
+        <v>1.15</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>22</v>
@@ -891,32 +909,26 @@
         <v>11</v>
       </c>
       <c r="E17" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="108.95" outlineLevel="0" r="18">
+      <c r="A18" s="1" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.35" outlineLevel="0" r="22">
-      <c r="A22" s="1" t="n">
-        <v>1.17</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.35" outlineLevel="0" r="23">
       <c r="A23" s="1" t="n">
-        <v>1.18</v>
+        <v>1.17</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>32</v>
@@ -925,15 +937,18 @@
         <v>33</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="24">
+      <c r="H23" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.35" outlineLevel="0" r="24">
       <c r="A24" s="1" t="n">
-        <v>1.19</v>
+        <v>1.18</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>32</v>
@@ -942,18 +957,15 @@
         <v>33</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H24" s="2" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="25">
       <c r="A25" s="1" t="n">
-        <v>1.2</v>
+        <v>1.19</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>32</v>
@@ -962,15 +974,18 @@
         <v>33</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="H25" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="26">
       <c r="A26" s="1" t="n">
-        <v>1.21</v>
+        <v>1.2</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>32</v>
@@ -979,18 +994,15 @@
         <v>33</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H26" s="2" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="27">
       <c r="A27" s="1" t="n">
-        <v>1.22</v>
+        <v>1.21</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>32</v>
@@ -999,7 +1011,7 @@
         <v>33</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>35</v>
@@ -1010,7 +1022,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="28">
       <c r="A28" s="1" t="n">
-        <v>1.23</v>
+        <v>1.22</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>32</v>
@@ -1019,7 +1031,7 @@
         <v>33</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>35</v>
@@ -1028,46 +1040,46 @@
         <v>42</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="37.3" outlineLevel="0" r="29">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="29">
       <c r="A29" s="1" t="n">
-        <v>1.24</v>
+        <v>1.23</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>32</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>47</v>
+        <v>35</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="37.3" outlineLevel="0" r="30">
       <c r="A30" s="1" t="n">
-        <v>1.25</v>
+        <v>1.24</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H30" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="73.1" outlineLevel="0" r="31">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="37.3" outlineLevel="0" r="31">
       <c r="A31" s="1" t="n">
-        <v>1.26</v>
+        <v>1.25</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>48</v>
@@ -1076,12 +1088,18 @@
         <v>49</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.35" outlineLevel="0" r="32">
+        <v>50</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="73.1" outlineLevel="0" r="32">
       <c r="A32" s="1" t="n">
-        <v>1.27</v>
+        <v>1.26</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>48</v>
@@ -1090,12 +1108,12 @@
         <v>49</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="61.15" outlineLevel="0" r="33">
+        <v>52</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.35" outlineLevel="0" r="33">
       <c r="A33" s="1" t="n">
-        <v>1.28</v>
+        <v>1.27</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>48</v>
@@ -1104,12 +1122,12 @@
         <v>49</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.35" outlineLevel="0" r="34">
+        <v>53</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="61.15" outlineLevel="0" r="34">
       <c r="A34" s="1" t="n">
-        <v>1.29</v>
+        <v>1.28</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>48</v>
@@ -1118,12 +1136,12 @@
         <v>49</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="49.25" outlineLevel="0" r="35">
+        <v>54</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.35" outlineLevel="0" r="35">
       <c r="A35" s="1" t="n">
-        <v>1.3</v>
+        <v>1.29</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>48</v>
@@ -1132,26 +1150,26 @@
         <v>49</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="37.3" outlineLevel="0" r="36">
+        <v>55</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="49.25" outlineLevel="0" r="36">
       <c r="A36" s="1" t="n">
-        <v>1.31</v>
+        <v>1.3</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>49</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.35" outlineLevel="0" r="37">
+        <v>56</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="37.3" outlineLevel="0" r="37">
       <c r="A37" s="1" t="n">
-        <v>1.32</v>
+        <v>1.31</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>57</v>
@@ -1160,29 +1178,26 @@
         <v>49</v>
       </c>
       <c r="E37" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.35" outlineLevel="0" r="38">
+      <c r="A38" s="1" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.35" outlineLevel="0" r="40">
-      <c r="A40" s="1" t="n">
-        <v>1.33</v>
-      </c>
-      <c r="B40" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C40" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.35" outlineLevel="0" r="41">
       <c r="A41" s="1" t="n">
-        <v>1.34</v>
+        <v>1.33</v>
       </c>
       <c r="B41" s="0" t="s">
         <v>48</v>
@@ -1191,12 +1206,15 @@
         <v>60</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="37.3" outlineLevel="0" r="42">
+        <v>61</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.35" outlineLevel="0" r="42">
       <c r="A42" s="1" t="n">
-        <v>1.35</v>
+        <v>1.34</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>48</v>
@@ -1205,15 +1223,12 @@
         <v>60</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I42" s="0" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="61.15" outlineLevel="0" r="43">
+        <v>63</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="37.3" outlineLevel="0" r="43">
       <c r="A43" s="1" t="n">
-        <v>1.36</v>
+        <v>1.35</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>48</v>
@@ -1222,12 +1237,15 @@
         <v>60</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="49.25" outlineLevel="0" r="44">
+        <v>64</v>
+      </c>
+      <c r="I43" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="61.15" outlineLevel="0" r="44">
       <c r="A44" s="1" t="n">
-        <v>1.37</v>
+        <v>1.36</v>
       </c>
       <c r="B44" s="0" t="s">
         <v>48</v>
@@ -1235,16 +1253,13 @@
       <c r="C44" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="D44" s="0" t="s">
-        <v>2</v>
-      </c>
       <c r="E44" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="37.3" outlineLevel="0" r="45">
+        <v>66</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="49.25" outlineLevel="0" r="45">
       <c r="A45" s="1" t="n">
-        <v>1.38</v>
+        <v>1.37</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>48</v>
@@ -1252,27 +1267,44 @@
       <c r="C45" s="0" t="s">
         <v>60</v>
       </c>
+      <c r="D45" s="0" t="s">
+        <v>2</v>
+      </c>
       <c r="E45" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="85.05" outlineLevel="0" r="46">
+        <v>67</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="37.3" outlineLevel="0" r="46">
       <c r="A46" s="1" t="n">
-        <v>1.39</v>
+        <v>1.38</v>
       </c>
       <c r="B46" s="0" t="s">
         <v>48</v>
       </c>
       <c r="C46" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="85.05" outlineLevel="0" r="47">
+      <c r="A47" s="1" t="n">
+        <v>1.39</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="E47" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="G47" s="2" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1292,16 +1324,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A:A"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="C1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="F25" activeCellId="0" pane="topLeft" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.2040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.2040816326531"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.1836734693878"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.7244897959184"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.6122448979592"/>
@@ -1314,422 +1345,479 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>73</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>81</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="2">
       <c r="A2" s="1" t="n">
-        <v>2.01</v>
+        <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="3">
       <c r="A3" s="1" t="n">
-        <v>2.02</v>
+        <v>1.01</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="4">
       <c r="A4" s="1" t="n">
-        <v>2.03</v>
+        <v>1.02</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="5">
       <c r="A5" s="1" t="n">
-        <v>2.04</v>
+        <v>1.03</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F5" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="6">
+      <c r="A6" s="1" t="n">
+        <v>1.04</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="G5" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="H5" s="0" t="s">
+      <c r="C6" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="I5" s="0" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="7">
+      <c r="E6" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="7">
       <c r="A7" s="1" t="n">
-        <v>2.05</v>
+        <v>2</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="E7" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="G7" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="F7" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>87</v>
-      </c>
       <c r="H7" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>78</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="8">
+      <c r="A8" s="1" t="n">
+        <v>2.01</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>103</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="9">
       <c r="A9" s="1" t="n">
-        <v>2.06</v>
+        <v>2.02</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="10">
       <c r="A10" s="1" t="n">
-        <v>2.07</v>
+        <v>2.03</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>98</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>74</v>
+        <v>83</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="11">
+        <v>107</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="11">
       <c r="A11" s="1" t="n">
-        <v>2.08</v>
+        <v>2.04</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>98</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>74</v>
+        <v>83</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="12">
       <c r="A12" s="1" t="n">
-        <v>2.09</v>
+        <v>2.05</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>98</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="13">
       <c r="A13" s="1" t="n">
-        <v>2.1</v>
+        <v>2.06</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>98</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>76</v>
+        <v>116</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="14">
+        <v>117</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="14">
       <c r="A14" s="1" t="n">
-        <v>2.11</v>
+        <v>2.07</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>98</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="15">
+        <v>120</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="15">
       <c r="A15" s="1" t="n">
-        <v>2.12</v>
+        <v>2.08</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>98</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="16">
+        <v>113</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="16">
       <c r="A16" s="1" t="n">
-        <v>2.13</v>
+        <v>2.09</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>98</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="17">
       <c r="A17" s="1" t="n">
-        <v>2.14</v>
+        <v>2.1</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>98</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>104</v>
+        <v>125</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="18">
       <c r="A18" s="1" t="n">
-        <v>2.15</v>
+        <v>2.11</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>98</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>74</v>
+        <v>126</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="19">
-      <c r="A19" s="1" t="n">
-        <v>2.16</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="E19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="G19" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="20">
-      <c r="A20" s="1" t="n">
-        <v>2.17</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="E20" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="H20" s="0" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1751,7 +1839,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A:A"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>

</xml_diff>